<commit_message>
ANA12: Added a section on Top Ten vulnerabilities plus some discussion. Also added some accompanying charts to the spreadsheet.
</commit_message>
<xml_diff>
--- a/Master Analysis.xlsx
+++ b/Master Analysis.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8745" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="3rdParty" sheetId="1" r:id="rId1"/>
     <sheet name="Source" sheetId="2" r:id="rId2"/>
+    <sheet name="Vuln per Lib Comparison" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3rdParty'!$A$1:$G$78</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="97">
   <si>
     <t>Project name</t>
   </si>
@@ -303,6 +304,12 @@
   </si>
   <si>
     <t>Diagram generator/data visualization</t>
+  </si>
+  <si>
+    <t>Vulnerabilities per third party library</t>
+  </si>
+  <si>
+    <t>Vulnerabilities per source library</t>
   </si>
 </sst>
 </file>
@@ -446,7 +453,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,8 +633,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -779,6 +798,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -824,7 +863,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -835,6 +874,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -896,6 +953,611 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerabilities per third party library</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>findbugs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mvnforum</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>heritrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gt2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>roller</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>marauroa</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>netbeans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tapestry</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jgrapht</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tomcat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vuln per Lib Comparison'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.1875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1153846153846101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.009009009009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50819672131147497</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.46296296296296202</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.34210526315789402</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33333333333333298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerabilities per source library</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>findbugs</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>mvnforum</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>heritrix</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gt2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>roller</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>marauroa</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>netbeans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tapestry</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>jgrapht</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tomcat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vuln per Lib Comparison'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66666666666666596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.144736842105263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.4977257959714096E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="46162304"/>
+        <c:axId val="46061440"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="46162304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="46061440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="46061440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="46162304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerabilities per source library</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$A$23:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>struts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tomcat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>hadoop</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rssowl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>heritrix</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jruby</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ireport</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>springframework</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>quartz</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>argouml</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vuln per Lib Comparison'!$B$23:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66666666666666596</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.44444444444444398</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19230769230769201</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16666666666666599</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.148148148148148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerabilities per third party library</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Vuln per Lib Comparison'!$A$23:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>struts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tomcat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>hadoop</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>rssowl</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>heritrix</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>jruby</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>ireport</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>springframework</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>quartz</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>argouml</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Vuln per Lib Comparison'!$C$23:$C$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33333333333300003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10204081632653</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.54545454545454E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1153846153846101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5555555555555497E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11627907</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="115144192"/>
+        <c:axId val="115145728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="115144192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115145728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="115145728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="115144192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>111124</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>124618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15874</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>134936</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>15874</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>42069</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1231,20 +1893,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3208,9 +3870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5136,4 +5798,338 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="34.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8">
+        <v>6.1875</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1.125</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1.1153846153846101</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1.009009009009</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0.144736842105263</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.50819672131147497</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.46296296296296202</v>
+      </c>
+      <c r="C8" s="8">
+        <v>6.4977257959714096E-3</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.34210526315789402</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="C11" s="12">
+        <v>3</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:4" s="14" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="9">
+        <v>3</v>
+      </c>
+      <c r="C24" s="9">
+        <v>0.33333333333300003</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.10204081632653</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <v>4.54545454545454E-2</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="C27" s="8">
+        <v>1.1153846153846101</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0.6</v>
+      </c>
+      <c r="C28" s="9">
+        <v>5.5555555555555497E-2</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="C29" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0.19230769230769201</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0.16666666666666599</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="12">
+        <v>0.148148148148148</v>
+      </c>
+      <c r="C32" s="12">
+        <v>0.11627907</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a Pie Chart indicating "Vulnerable vs Non-Vulnerable" projects. This gives an indication of the percentage of projects that have vulnerabilities in their third party libraries versus source party libraries.
This will probably make a good opening examination of the data.
</commit_message>
<xml_diff>
--- a/Master Analysis.xlsx
+++ b/Master Analysis.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="3rdParty" sheetId="1" r:id="rId1"/>
     <sheet name="Source" sheetId="2" r:id="rId2"/>
     <sheet name="Vuln per Lib Comparison" sheetId="3" r:id="rId3"/>
+    <sheet name="Vulnerable vs Non-Vulnerable" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3rdParty'!$A$1:$G$77</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="107">
   <si>
     <t>Project name</t>
   </si>
@@ -334,6 +335,12 @@
   </si>
   <si>
     <t>games</t>
+  </si>
+  <si>
+    <t>Vulnerable:</t>
+  </si>
+  <si>
+    <t>Not Vulnerable:</t>
   </si>
 </sst>
 </file>
@@ -670,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -842,6 +849,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -887,7 +938,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -917,6 +968,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1195,11 +1250,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116239360"/>
-        <c:axId val="116732672"/>
+        <c:axId val="115264512"/>
+        <c:axId val="115352320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116239360"/>
+        <c:axId val="115264512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,7 +1263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116732672"/>
+        <c:crossAx val="115352320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1216,7 +1271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116732672"/>
+        <c:axId val="115352320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116239360"/>
+        <c:crossAx val="115264512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1274,7 +1329,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Vuln per Lib Comparison'!$B$22</c:f>
+              <c:f>'Vuln per Lib Comparison'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1285,7 +1340,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Vuln per Lib Comparison'!$A$23:$A$32</c:f>
+              <c:f>'Vuln per Lib Comparison'!$A$21:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1323,7 +1378,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Vuln per Lib Comparison'!$B$23:$B$32</c:f>
+              <c:f>'Vuln per Lib Comparison'!$B$21:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1367,7 +1422,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Vuln per Lib Comparison'!$C$22</c:f>
+              <c:f>'Vuln per Lib Comparison'!$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1378,7 +1433,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'Vuln per Lib Comparison'!$A$23:$A$32</c:f>
+              <c:f>'Vuln per Lib Comparison'!$A$21:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1416,7 +1471,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Vuln per Lib Comparison'!$C$23:$C$32</c:f>
+              <c:f>'Vuln per Lib Comparison'!$C$21:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1465,11 +1520,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116757632"/>
-        <c:axId val="116759168"/>
+        <c:axId val="115385472"/>
+        <c:axId val="115387008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116757632"/>
+        <c:axId val="115385472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1533,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116759168"/>
+        <c:crossAx val="115387008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1486,7 +1541,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116759168"/>
+        <c:axId val="115387008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1497,7 +1552,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116757632"/>
+        <c:crossAx val="115385472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1519,6 +1574,255 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Third</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Party Libraries</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'3rdParty'!$A$90:$A$91</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable:</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not Vulnerable:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3rdParty'!$B$90:$B$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Source Libraries</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Source!$A$90:$A$91</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Vulnerable:</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not Vulnerable:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Source!$B$90:$B$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1526,13 +1830,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>111124</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>124618</xdr:rowOff>
+      <xdr:rowOff>67468</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>15874</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1554,19 +1858,86 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>134936</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180181</xdr:rowOff>
+      <xdr:colOff>115886</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>46831</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>15874</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>42069</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>606424</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>89694</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>69849</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1606,7 +1977,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:H77" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:H77"/>
+  <autoFilter ref="A1:H77">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:H78">
     <sortCondition ref="A1:A78"/>
   </sortState>
@@ -1911,22 +2288,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2:H77"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3933,56 +4310,74 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B81" s="3">
         <f>COUNTIF(B2:B77,TRUE)</f>
         <v>39</v>
       </c>
-      <c r="C82" s="3">
-        <f>SUM(C2:C81)</f>
+      <c r="C81" s="3">
+        <f>SUM(C2:C80)</f>
         <v>839</v>
       </c>
-      <c r="D82" s="3">
-        <f>SUM(D2:D81)</f>
+      <c r="D81" s="3">
+        <f>SUM(D2:D80)</f>
         <v>661</v>
       </c>
-      <c r="E82" s="3">
+      <c r="E81" s="3">
         <f>SUM(E2:E77)</f>
         <v>2357</v>
       </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="4">
-        <f>SUM(G2:G81)</f>
+      <c r="F81" s="3"/>
+      <c r="G81" s="4">
+        <f>SUM(G2:G80)</f>
         <v>237</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3">
+      <c r="B84" s="3"/>
+      <c r="C84" s="3">
         <f>AVERAGE(C2:C77)</f>
         <v>11.039473684210526</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D84" s="3">
         <f>AVERAGE(D2:D77)</f>
         <v>8.6973684210526319</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E84" s="3">
         <f>AVERAGE(E2:E77)</f>
         <v>31.013157894736842</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F84" s="3">
         <f>AVERAGE(F2:F77)</f>
         <v>0.20780923970191487</v>
       </c>
-      <c r="G85" s="4">
+      <c r="G84" s="4">
         <f>AVERAGE(G2:G77)</f>
         <v>3.1184210526315788</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90" s="16">
+        <f>COUNTIF(B2:B77,TRUE)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" s="18">
+        <f>COUNTIF(B2:B77,FALSE)</f>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3996,22 +4391,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A90" sqref="A90:B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -4042,7 +4437,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4068,7 +4463,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4094,7 +4489,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4146,7 +4541,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4172,7 +4567,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -4198,7 +4593,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -4224,7 +4619,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -4250,7 +4645,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -4276,7 +4671,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -4302,7 +4697,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -4328,7 +4723,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -4354,7 +4749,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -4380,7 +4775,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -4406,7 +4801,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -4458,7 +4853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -4484,7 +4879,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -4510,7 +4905,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -4536,7 +4931,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -4562,7 +4957,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -4588,7 +4983,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -4614,7 +5009,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -4640,7 +5035,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -4744,7 +5139,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -4770,7 +5165,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -4796,7 +5191,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -4822,7 +5217,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -4874,7 +5269,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -4900,7 +5295,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -4926,7 +5321,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -4978,7 +5373,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -5004,7 +5399,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -5030,7 +5425,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -5056,7 +5451,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -5082,7 +5477,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -5108,7 +5503,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -5134,7 +5529,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -5160,7 +5555,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -5186,7 +5581,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -5212,7 +5607,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -5238,7 +5633,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -5290,7 +5685,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -5316,7 +5711,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -5342,7 +5737,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -5368,7 +5763,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -5394,7 +5789,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -5420,7 +5815,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -5472,7 +5867,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -5498,7 +5893,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -5524,7 +5919,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -5576,7 +5971,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -5602,7 +5997,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -5628,7 +6023,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -5680,7 +6075,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -5732,7 +6127,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -5784,7 +6179,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -5836,7 +6231,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -5888,7 +6283,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -5914,7 +6309,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -5940,7 +6335,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -5966,7 +6361,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -5992,7 +6387,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -6018,56 +6413,74 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B81" s="3">
         <f>COUNTIF(B2:B77,TRUE)</f>
         <v>15</v>
       </c>
-      <c r="C82" s="3">
-        <f>SUM(C2:C81)</f>
+      <c r="C81" s="3">
+        <f>SUM(C2:C80)</f>
         <v>438</v>
       </c>
-      <c r="D82" s="3">
-        <f>SUM(D2:D81)</f>
+      <c r="D81" s="3">
+        <f>SUM(D2:D80)</f>
         <v>115</v>
       </c>
-      <c r="E82" s="3">
+      <c r="E81" s="3">
         <f>SUM(E2:E77)</f>
         <v>2381</v>
       </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="4">
-        <f>SUM(G2:G81)</f>
+      <c r="F81" s="3"/>
+      <c r="G81" s="4">
+        <f>SUM(G2:G80)</f>
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3">
+      <c r="B84" s="3"/>
+      <c r="C84" s="3">
         <f>AVERAGE(C2:C77)</f>
         <v>5.7631578947368425</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D84" s="3">
         <f>AVERAGE(D2:D77)</f>
         <v>1.513157894736842</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E84" s="3">
         <f>AVERAGE(E2:E77)</f>
         <v>31.328947368421051</v>
       </c>
-      <c r="F85" s="3">
+      <c r="F84" s="3">
         <f>AVERAGE(F2:F77)</f>
         <v>0.15701649929243686</v>
       </c>
-      <c r="G85" s="4">
+      <c r="G84" s="4">
         <f>AVERAGE(G2:G77)</f>
         <v>2.6842105263157894</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90" s="16">
+        <f>COUNTIF(B2:B77,TRUE)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B91" s="18">
+        <f>COUNTIF(B2:B77,FALSE)</f>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -6083,8 +6496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6248,30 +6661,58 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:4" s="14" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="7" t="s">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="9">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9">
+        <v>0.33333333333300003</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="B23" s="8">
-        <v>4.4000000000000004</v>
+        <v>1</v>
       </c>
       <c r="C23" s="8">
-        <v>0.27500000000000002</v>
+        <v>0.10204081632653</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>91</v>
@@ -6279,127 +6720,99 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B24" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" s="9">
-        <v>0.33333333333300003</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>91</v>
+        <v>4.54545454545454E-2</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" s="8">
-        <v>1</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="C25" s="8">
-        <v>0.10204081632653</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>91</v>
+        <v>1.1153846153846101</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B26" s="9">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C26" s="9">
-        <v>4.54545454545454E-2</v>
+        <v>5.5555555555555497E-2</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B27" s="8">
-        <v>0.66666666666666596</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="C27" s="8">
-        <v>1.1153846153846101</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>88</v>
+        <v>0.125</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="B28" s="9">
-        <v>0.6</v>
+        <v>0.19230769230769201</v>
       </c>
       <c r="C28" s="9">
-        <v>5.5555555555555497E-2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B29" s="8">
-        <v>0.44444444444444398</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="C29" s="8">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="9">
-        <v>0.19230769230769201</v>
-      </c>
-      <c r="C30" s="9">
-        <v>0</v>
-      </c>
-      <c r="D30" s="9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0.16666666666666599</v>
-      </c>
-      <c r="C31" s="8">
-        <v>0</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12" t="s">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B30" s="12">
         <v>0.148148148148148</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C30" s="12">
         <v>0.11627907</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>93</v>
       </c>
     </row>
@@ -6411,4 +6824,19 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ANA1: Added information on the outliers from the 2nd Analysis Phase. This covered GeoTools, Findbugs and NetBeans.
</commit_message>
<xml_diff>
--- a/Master Analysis.xlsx
+++ b/Master Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="3rdParty" sheetId="1" r:id="rId1"/>
@@ -1250,11 +1250,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115264512"/>
-        <c:axId val="115352320"/>
+        <c:axId val="117632384"/>
+        <c:axId val="117777536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115264512"/>
+        <c:axId val="117632384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115352320"/>
+        <c:crossAx val="117777536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1271,7 +1271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115352320"/>
+        <c:axId val="117777536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,14 +1282,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115264512"/>
+        <c:crossAx val="117632384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1520,11 +1519,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115385472"/>
-        <c:axId val="115387008"/>
+        <c:axId val="117818880"/>
+        <c:axId val="117820416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="115385472"/>
+        <c:axId val="117818880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1533,7 +1532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115387008"/>
+        <c:crossAx val="117820416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1541,7 +1540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="115387008"/>
+        <c:axId val="117820416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,14 +1551,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115385472"/>
+        <c:crossAx val="117818880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1958,8 +1956,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H77" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:H77"/>
-  <sortState ref="A2:H78">
-    <sortCondition ref="A1:A78"/>
+  <sortState ref="A2:H77">
+    <sortCondition descending="1" ref="D1:D77"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Project name"/>
@@ -2290,9 +2288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,839 +2334,839 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>270</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.46296296296296202</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>96</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>112</v>
+      </c>
+      <c r="D3">
+        <v>112</v>
+      </c>
+      <c r="E3">
+        <v>111</v>
+      </c>
+      <c r="F3">
+        <v>1.009009009009</v>
+      </c>
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="H3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="E4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>6.1875</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>58</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>1.125</v>
+      </c>
+      <c r="G5">
         <v>5</v>
       </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>43</v>
-      </c>
-      <c r="F5">
-        <v>0.116279069767441</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>98</v>
+      <c r="H5" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>0.50819672131147497</v>
+      </c>
+      <c r="G6">
         <v>6</v>
       </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>99</v>
+      <c r="H6" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1.1153846153846101</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F8">
-        <v>0.10204081632653</v>
+        <v>0.26315789473684198</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>0.31506849315068403</v>
+      </c>
+      <c r="G9">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>17</v>
-      </c>
-      <c r="F9">
-        <v>0.17647058823529399</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
       <c r="H9" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.12707182320441901</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>9.71428571428571E-2</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E12">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.34210526315789402</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>102</v>
+        <v>4</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="D14">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E14">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="F14">
-        <v>9.71428571428571E-2</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G14">
-        <v>85</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B15" t="b">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="F15">
-        <v>2.8571428571428501E-2</v>
+        <v>0.12676056338028099</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.146341463414634</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="F17">
-        <v>0.31506849315068403</v>
+        <v>0.116279069767441</v>
       </c>
       <c r="G17">
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.10204081632653</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F19">
-        <v>6.1875</v>
+        <v>0.11111111111111099</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>86</v>
+      <c r="H19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="F20">
-        <v>0.1</v>
+        <v>0.10204081632653</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="F21">
-        <v>0.30769230769230699</v>
+        <v>0.11363636363636299</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E22">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.30769230769230699</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="F23">
-        <v>0.11111111111111099</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
       </c>
       <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>21</v>
+      </c>
+      <c r="F24">
+        <v>0.19047619047618999</v>
+      </c>
+      <c r="G24">
         <v>2</v>
       </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24">
-        <v>65</v>
-      </c>
-      <c r="F24">
-        <v>3.0769230769230702E-2</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
       <c r="H24" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F25">
-        <v>0.115384615384615</v>
+        <v>0.25</v>
       </c>
       <c r="G25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
       </c>
       <c r="C26">
-        <v>112</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>112</v>
+        <v>3</v>
       </c>
       <c r="E26">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="F26">
-        <v>1.009009009009</v>
+        <v>0.17647058823529399</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="F27">
-        <v>0.10204081632653</v>
+        <v>0.115384615384615</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F28">
-        <v>1.1153846153846101</v>
+        <v>9.375E-2</v>
       </c>
       <c r="G28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>54</v>
+      </c>
+      <c r="F29">
+        <v>5.5555555555555497E-2</v>
+      </c>
+      <c r="G29">
         <v>2</v>
       </c>
-      <c r="E29">
-        <v>17</v>
-      </c>
-      <c r="F29">
-        <v>0.11764705882352899</v>
-      </c>
-      <c r="G29">
-        <v>5</v>
-      </c>
       <c r="H29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>6.6666666666666596E-2</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>9.375E-2</v>
+        <v>0.5</v>
       </c>
       <c r="G31">
-        <v>4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>102</v>
+        <v>1</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E32">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="F32">
-        <v>0.22222222222222199</v>
+        <v>3.0769230769230702E-2</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E33">
-        <v>88</v>
+        <v>17</v>
       </c>
       <c r="F33">
-        <v>0.125</v>
+        <v>0.11764705882352899</v>
       </c>
       <c r="G33">
         <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -3177,180 +3175,180 @@
         <v>4</v>
       </c>
       <c r="D34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F34">
-        <v>0.19047619047618999</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
-      <c r="H34" t="s">
-        <v>103</v>
+      <c r="H34" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
       </c>
       <c r="C35">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E35">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="F35">
-        <v>0.12676056338028099</v>
+        <v>4.1666666666666602E-2</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H35" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>4.54545454545454E-2</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>181</v>
+        <v>35</v>
       </c>
       <c r="F37">
-        <v>0.12707182320441901</v>
+        <v>2.8571428571428501E-2</v>
       </c>
       <c r="G37">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>1.3698630136986301E-2</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40" t="s">
-        <v>101</v>
+        <v>1</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B41" t="b">
         <v>0</v>
@@ -3362,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -3371,12 +3369,12 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B42" t="b">
         <v>0</v>
@@ -3388,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -3397,38 +3395,38 @@
         <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="B43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F43">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
@@ -3440,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -3449,12 +3447,12 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="B45" t="b">
         <v>0</v>
@@ -3466,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -3475,38 +3473,38 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="B46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="F46">
-        <v>4.1666666666666602E-2</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B47" t="b">
         <v>0</v>
@@ -3518,7 +3516,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -3527,12 +3525,12 @@
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B48" t="b">
         <v>0</v>
@@ -3544,7 +3542,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -3553,90 +3551,90 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>5.5555555555555497E-2</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F50">
-        <v>0.146341463414634</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="F51">
-        <v>6.6666666666666596E-2</v>
+        <v>0</v>
       </c>
       <c r="G51">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -3648,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -3657,12 +3655,12 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
@@ -3674,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -3683,12 +3681,12 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
@@ -3700,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -3709,116 +3707,116 @@
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="F55">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>1</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>89</v>
+        <v>0</v>
+      </c>
+      <c r="H55" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="F56">
-        <v>1.3698630136986301E-2</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F57">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>1.125</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>5</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="H58" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B59" t="b">
         <v>0</v>
@@ -3830,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -3839,38 +3837,38 @@
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="B60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>270</v>
+        <v>9</v>
       </c>
       <c r="F60">
-        <v>0.46296296296296202</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>14</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
@@ -3882,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -3891,12 +3889,12 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B62" t="b">
         <v>0</v>
@@ -3908,7 +3906,7 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -3917,12 +3915,12 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B63" t="b">
         <v>0</v>
@@ -3934,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -3943,12 +3941,12 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B64" t="b">
         <v>0</v>
@@ -3960,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -3974,59 +3972,59 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B65" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="F65">
-        <v>0.50819672131147497</v>
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>6</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="H65" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>4.54545454545454E-2</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B67" t="b">
         <v>0</v>
@@ -4038,7 +4036,7 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -4052,7 +4050,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B68" t="b">
         <v>0</v>
@@ -4064,7 +4062,7 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -4078,111 +4076,111 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F69">
-        <v>0.11363636363636299</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B70" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="F70">
-        <v>0.27500000000000002</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B71" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C71">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="F71">
-        <v>0.34210526315789402</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>4</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>91</v>
+        <v>0</v>
+      </c>
+      <c r="H71" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>1</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>91</v>
+        <v>0</v>
+      </c>
+      <c r="H72" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B73" t="b">
         <v>0</v>
@@ -4194,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -4203,33 +4201,33 @@
         <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="F74">
-        <v>0.26315789473684198</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H74" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4355,7 +4353,7 @@
       </c>
       <c r="F84" s="3">
         <f>AVERAGE(F2:F77)</f>
-        <v>0.20780923970191487</v>
+        <v>0.20780923970191489</v>
       </c>
       <c r="G84" s="4">
         <f>AVERAGE(G2:G77)</f>
@@ -6830,7 +6828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DA12: Added some information on design, in particular about the analysis strategies that were used. Also some minor tidy-up work of the document, including the addition of the Appendix of all projects used.
</commit_message>
<xml_diff>
--- a/Master Analysis.xlsx
+++ b/Master Analysis.xlsx
@@ -1250,11 +1250,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="117632384"/>
-        <c:axId val="117777536"/>
+        <c:axId val="70354432"/>
+        <c:axId val="70355968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117632384"/>
+        <c:axId val="70354432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117777536"/>
+        <c:crossAx val="70355968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1271,7 +1271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117777536"/>
+        <c:axId val="70355968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,7 +1282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117632384"/>
+        <c:crossAx val="70354432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1519,11 +1519,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="117818880"/>
-        <c:axId val="117820416"/>
+        <c:axId val="70385024"/>
+        <c:axId val="102499456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117818880"/>
+        <c:axId val="70385024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,7 +1532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117820416"/>
+        <c:crossAx val="102499456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1540,7 +1540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117820416"/>
+        <c:axId val="102499456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117818880"/>
+        <c:crossAx val="70385024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1607,7 +1607,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1729,7 +1728,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1956,8 +1954,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H77" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:H77"/>
-  <sortState ref="A2:H77">
-    <sortCondition descending="1" ref="D1:D77"/>
+  <sortState ref="A5:H74">
+    <sortCondition ref="A1:A77"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Project name"/>
@@ -2289,8 +2287,8 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,839 +2332,839 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>270</v>
+        <v>3</v>
       </c>
       <c r="F2">
-        <v>0.46296296296296202</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>112</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>1.009009009009</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4">
-        <v>6.1875</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>86</v>
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F5">
-        <v>1.125</v>
+        <v>0.116279069767441</v>
       </c>
       <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>88</v>
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.50819672131147497</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1.1153846153846101</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="F8">
-        <v>0.26315789473684198</v>
+        <v>0.10204081632653</v>
       </c>
       <c r="G8">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>17</v>
       </c>
-      <c r="B9" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <v>73</v>
-      </c>
       <c r="F9">
-        <v>0.31506849315068403</v>
+        <v>0.17647058823529399</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="B10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>181</v>
+        <v>7</v>
       </c>
       <c r="F10">
-        <v>0.12707182320441901</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>175</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>9.71428571428571E-2</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F12">
-        <v>0.34210526315789402</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>91</v>
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B14" t="b">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E14">
-        <v>40</v>
+        <v>175</v>
       </c>
       <c r="F14">
-        <v>0.27500000000000002</v>
+        <v>9.71428571428571E-2</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
         <v>35</v>
       </c>
-      <c r="B15" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>9</v>
-      </c>
-      <c r="D15">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>71</v>
-      </c>
       <c r="F15">
-        <v>0.12676056338028099</v>
+        <v>2.8571428571428501E-2</v>
       </c>
       <c r="G15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="F16">
-        <v>0.146341463414634</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="E17">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="F17">
-        <v>0.116279069767441</v>
+        <v>0.31506849315068403</v>
       </c>
       <c r="G17">
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>0.10204081632653</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B19" t="b">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="E19">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F19">
-        <v>0.11111111111111099</v>
+        <v>6.1875</v>
       </c>
       <c r="G19">
         <v>2</v>
       </c>
-      <c r="H19" t="s">
-        <v>98</v>
+      <c r="H19" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B20" t="b">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F20">
-        <v>0.10204081632653</v>
+        <v>0.1</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B21" t="b">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="F21">
-        <v>0.11363636363636299</v>
+        <v>0.30769230769230699</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F22">
-        <v>0.30769230769230699</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B23" t="b">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F23">
-        <v>0.22222222222222199</v>
+        <v>0.11111111111111099</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B24" t="b">
         <v>1</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="F24">
-        <v>0.19047619047618999</v>
+        <v>3.0769230769230702E-2</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B25" t="b">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E25">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F25">
-        <v>0.25</v>
+        <v>0.115384615384615</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
       </c>
       <c r="C26">
+        <v>112</v>
+      </c>
+      <c r="D26">
+        <v>112</v>
+      </c>
+      <c r="E26">
+        <v>111</v>
+      </c>
+      <c r="F26">
+        <v>1.009009009009</v>
+      </c>
+      <c r="G26">
         <v>3</v>
       </c>
-      <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26">
-        <v>17</v>
-      </c>
-      <c r="F26">
-        <v>0.17647058823529399</v>
-      </c>
-      <c r="G26">
-        <v>1</v>
-      </c>
       <c r="H26" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F27">
-        <v>0.115384615384615</v>
+        <v>0.10204081632653</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D28">
+        <v>29</v>
+      </c>
+      <c r="E28">
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <v>1.1153846153846101</v>
+      </c>
+      <c r="G28">
         <v>3</v>
       </c>
-      <c r="E28">
-        <v>32</v>
-      </c>
-      <c r="F28">
-        <v>9.375E-2</v>
-      </c>
-      <c r="G28">
-        <v>4</v>
-      </c>
       <c r="H28" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B29" t="b">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="F29">
-        <v>5.5555555555555497E-2</v>
+        <v>0.11764705882352899</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>6.6666666666666596E-2</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="B31" t="b">
         <v>1</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F31">
-        <v>0.5</v>
+        <v>9.375E-2</v>
       </c>
       <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>89</v>
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B32" t="b">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E32">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="F32">
-        <v>3.0769230769230702E-2</v>
+        <v>0.22222222222222199</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
       </c>
       <c r="C33">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E33">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="F33">
-        <v>0.11764705882352899</v>
+        <v>0.125</v>
       </c>
       <c r="G33">
         <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B34" t="b">
         <v>1</v>
@@ -3175,180 +3173,180 @@
         <v>4</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E34">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F34">
-        <v>0.33333333333333298</v>
+        <v>0.19047619047618999</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>88</v>
+      <c r="H34" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B35" t="b">
         <v>1</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E35">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="F35">
-        <v>4.1666666666666602E-2</v>
+        <v>0.12676056338028099</v>
       </c>
       <c r="G35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H35" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="B36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="F36">
-        <v>4.54545454545454E-2</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E37">
-        <v>35</v>
+        <v>181</v>
       </c>
       <c r="F37">
-        <v>2.8571428571428501E-2</v>
+        <v>0.12707182320441901</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="H37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F38">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>1.3698630136986301E-2</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F40">
-        <v>0.33333333333333298</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>91</v>
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="B41" t="b">
         <v>0</v>
@@ -3360,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -3369,12 +3367,12 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="B42" t="b">
         <v>0</v>
@@ -3386,7 +3384,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -3395,38 +3393,38 @@
         <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43">
         <v>4</v>
       </c>
-      <c r="B43" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
       <c r="D43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E43">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="s">
-        <v>97</v>
+        <v>2</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B44" t="b">
         <v>0</v>
@@ -3438,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -3447,12 +3445,12 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B45" t="b">
         <v>0</v>
@@ -3464,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -3473,38 +3471,38 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E46">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>4.1666666666666602E-2</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B47" t="b">
         <v>0</v>
@@ -3516,7 +3514,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -3525,12 +3523,12 @@
         <v>0</v>
       </c>
       <c r="H47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B48" t="b">
         <v>0</v>
@@ -3542,7 +3540,7 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -3551,90 +3549,90 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>5.5555555555555497E-2</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H49" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E50">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>0.146341463414634</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>6.6666666666666596E-2</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -3646,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -3655,12 +3653,12 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B53" t="b">
         <v>0</v>
@@ -3672,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -3681,12 +3679,12 @@
         <v>0</v>
       </c>
       <c r="H53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
@@ -3698,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -3707,116 +3705,116 @@
         <v>0</v>
       </c>
       <c r="H54" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="B55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E55">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55" t="s">
-        <v>87</v>
+        <v>1</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1.3698630136986301E-2</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E57">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>1.125</v>
       </c>
       <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58" t="s">
-        <v>87</v>
+        <v>5</v>
+      </c>
+      <c r="H58" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B59" t="b">
         <v>0</v>
@@ -3828,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -3837,38 +3835,38 @@
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E60">
-        <v>9</v>
+        <v>270</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>0.46296296296296202</v>
       </c>
       <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60" t="s">
-        <v>103</v>
+        <v>14</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B61" t="b">
         <v>0</v>
@@ -3880,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -3889,12 +3887,12 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="B62" t="b">
         <v>0</v>
@@ -3906,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -3915,12 +3913,12 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B63" t="b">
         <v>0</v>
@@ -3932,7 +3930,7 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -3941,12 +3939,12 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B64" t="b">
         <v>0</v>
@@ -3958,7 +3956,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -3972,59 +3970,59 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E65">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>0.50819672131147497</v>
       </c>
       <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65" t="s">
-        <v>98</v>
+        <v>6</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>4.54545454545454E-2</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H66" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B67" t="b">
         <v>0</v>
@@ -4036,7 +4034,7 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -4050,7 +4048,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B68" t="b">
         <v>0</v>
@@ -4062,7 +4060,7 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -4076,111 +4074,111 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E69">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>0.11363636363636299</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E70">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H70" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E71">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>0.34210526315789402</v>
       </c>
       <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71" t="s">
-        <v>101</v>
+        <v>4</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72" t="s">
-        <v>96</v>
+        <v>1</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B73" t="b">
         <v>0</v>
@@ -4192,7 +4190,7 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -4201,33 +4199,33 @@
         <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E74">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>0.26315789473684198</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H74" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4353,7 +4351,7 @@
       </c>
       <c r="F84" s="3">
         <f>AVERAGE(F2:F77)</f>
-        <v>0.20780923970191489</v>
+        <v>0.20780923970191487</v>
       </c>
       <c r="G84" s="4">
         <f>AVERAGE(G2:G77)</f>

</xml_diff>

<commit_message>
ANA13: Add a section on the top ten projects which have libraries with the most vulnerabilities GEW4: Added a section on all the various tools that were used to help complete the project.
</commit_message>
<xml_diff>
--- a/Master Analysis.xlsx
+++ b/Master Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="10230" windowHeight="8730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="3rdParty" sheetId="1" r:id="rId1"/>
@@ -1250,11 +1250,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70354432"/>
-        <c:axId val="70355968"/>
+        <c:axId val="126807424"/>
+        <c:axId val="126960768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70354432"/>
+        <c:axId val="126807424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70355968"/>
+        <c:crossAx val="126960768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1271,7 +1271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70355968"/>
+        <c:axId val="126960768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1282,7 +1282,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70354432"/>
+        <c:crossAx val="126807424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1519,11 +1519,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="70385024"/>
-        <c:axId val="102499456"/>
+        <c:axId val="126985728"/>
+        <c:axId val="126987264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70385024"/>
+        <c:axId val="126985728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1532,7 +1532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102499456"/>
+        <c:crossAx val="126987264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1540,7 +1540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102499456"/>
+        <c:axId val="126987264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1551,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70385024"/>
+        <c:crossAx val="126985728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1979,9 +1979,12 @@
         <filter val="TRUE"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="6">
+      <top10 val="10" filterVal="2"/>
+    </filterColumn>
   </autoFilter>
-  <sortState ref="A2:H78">
-    <sortCondition ref="A1:A78"/>
+  <sortState ref="A5:H72">
+    <sortCondition descending="1" ref="G1:G77"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" name="Project name"/>
@@ -2286,8 +2289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -4389,19 +4392,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A90" sqref="A90:B91"/>
+      <selection pane="bottomLeft" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -4513,28 +4516,28 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>27</v>
+        <v>342</v>
       </c>
       <c r="F5">
-        <v>0.148148148148148</v>
+        <v>5.84795321637426E-3</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -4825,28 +4828,28 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>126</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>342</v>
+        <v>52</v>
       </c>
       <c r="F17">
-        <v>5.84795321637426E-3</v>
+        <v>0.115384615384615</v>
       </c>
       <c r="G17">
-        <v>123</v>
+        <v>38</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -5059,80 +5062,80 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B26" t="b">
         <v>1</v>
       </c>
       <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>1539</v>
+      </c>
+      <c r="F26">
+        <v>6.4977257959714096E-3</v>
+      </c>
+      <c r="G26">
         <v>11</v>
       </c>
-      <c r="D26">
-        <v>11</v>
-      </c>
-      <c r="E26">
-        <v>76</v>
-      </c>
-      <c r="F26">
-        <v>0.144736842105263</v>
-      </c>
-      <c r="G26">
-        <v>5</v>
-      </c>
-      <c r="H26" t="s">
-        <v>87</v>
+      <c r="H26" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="B27" t="b">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>148</v>
       </c>
       <c r="D27">
+        <v>39</v>
+      </c>
+      <c r="E27">
+        <v>13</v>
+      </c>
+      <c r="F27">
         <v>3</v>
       </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
       <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="H27" t="s">
-        <v>101</v>
+        <v>6</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" t="b">
         <v>1</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="F28">
-        <v>0.66666666666666596</v>
+        <v>0.144736842105263</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -5241,28 +5244,28 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="B33" t="b">
         <v>1</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="D33">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E33">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F33">
-        <v>0.44444444444444398</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -5345,28 +5348,28 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
       </c>
       <c r="C37">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E37">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="F37">
-        <v>0.115384615384615</v>
+        <v>0.6</v>
       </c>
       <c r="G37">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -5657,28 +5660,28 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B49" t="b">
         <v>1</v>
       </c>
       <c r="C49">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>47</v>
+      </c>
+      <c r="F49">
+        <v>4.2553191489361701E-2</v>
+      </c>
+      <c r="G49">
         <v>3</v>
       </c>
-      <c r="E49">
-        <v>5</v>
-      </c>
-      <c r="F49">
-        <v>0.6</v>
-      </c>
-      <c r="G49">
-        <v>4</v>
-      </c>
       <c r="H49" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -5839,28 +5842,28 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="B56" t="b">
         <v>1</v>
       </c>
       <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
         <v>3</v>
       </c>
-      <c r="D56">
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
         <v>2</v>
       </c>
-      <c r="E56">
-        <v>47</v>
-      </c>
-      <c r="F56">
-        <v>4.2553191489361701E-2</v>
-      </c>
-      <c r="G56">
-        <v>3</v>
-      </c>
       <c r="H56" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -5943,28 +5946,28 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B60" t="b">
         <v>1</v>
       </c>
       <c r="C60">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D60">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E60">
-        <v>1539</v>
+        <v>9</v>
       </c>
       <c r="F60">
-        <v>6.4977257959714096E-3</v>
+        <v>0.44444444444444398</v>
       </c>
       <c r="G60">
-        <v>11</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>90</v>
+        <v>2</v>
+      </c>
+      <c r="H60" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -6045,30 +6048,30 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="B64" t="b">
         <v>1</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="F64">
-        <v>0.16666666666666599</v>
+        <v>0.148148148148148</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="H64" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -6097,30 +6100,30 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B66" t="b">
         <v>1</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>0.66666666666666596</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -6149,24 +6152,24 @@
         <v>96</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B68" t="b">
         <v>1</v>
       </c>
       <c r="C68">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F68">
-        <v>0.19230769230769201</v>
+        <v>0.16666666666666599</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -6201,30 +6204,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B70" t="b">
         <v>1</v>
       </c>
       <c r="C70">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F70">
-        <v>4.4000000000000004</v>
+        <v>1</v>
       </c>
       <c r="G70">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H70" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -6253,30 +6256,30 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B72" t="b">
         <v>1</v>
       </c>
       <c r="C72">
-        <v>148</v>
+        <v>5</v>
       </c>
       <c r="D72">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="E72">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F72">
-        <v>3</v>
+        <v>0.19230769230769201</v>
       </c>
       <c r="G72">
-        <v>6</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>91</v>
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>